<commit_message>
Continuação do movimento circular e animação
</commit_message>
<xml_diff>
--- a/Parte 2/Dados/bloco_rampa.xlsx
+++ b/Parte 2/Dados/bloco_rampa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26c96ee5941d8100/USP/3_Semestre/MAC0209/EP1/MAC0209-EP1/Parte 2/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="563" documentId="8_{CC4223DC-985D-49C7-BAC9-916EC20BBDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C3D9B67-DD7A-484A-A2B6-C1EA258C4042}"/>
+  <xr:revisionPtr revIDLastSave="584" documentId="8_{CC4223DC-985D-49C7-BAC9-916EC20BBDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE9CE1F6-E346-460C-88C8-A34D4E29820D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -213,7 +213,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,6 +241,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -488,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -587,8 +593,41 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -597,15 +636,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -629,32 +659,16 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -662,30 +676,84 @@
   </cellStyles>
   <dxfs count="58">
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -761,63 +829,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
@@ -825,20 +836,23 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1809,10 +1823,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73A78A46-A924-4579-9890-5F61199F6EAF}" name="Tabela1" displayName="Tabela1" ref="B6:C10" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54" totalsRowBorderDxfId="53">
   <autoFilter ref="B6:C10" xr:uid="{73A78A46-A924-4579-9890-5F61199F6EAF}"/>
@@ -1900,22 +1910,22 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{0EEF875D-95AE-4ACD-85BA-45A6EC0C78C0}" name="Tabela7" displayName="Tabela7" ref="B14:C19" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{0EEF875D-95AE-4ACD-85BA-45A6EC0C78C0}" name="Tabela7" displayName="Tabela7" ref="B14:C19" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="B14:C19" xr:uid="{0EEF875D-95AE-4ACD-85BA-45A6EC0C78C0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F624ECCE-44BF-418C-8DBF-94BFECE11FC0}" name="Frequência" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{835B37EF-3836-43EB-AA97-DF2721F2F841}" name="Valor" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{F624ECCE-44BF-418C-8DBF-94BFECE11FC0}" name="Frequência" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{835B37EF-3836-43EB-AA97-DF2721F2F841}" name="Valor" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F4D0B40F-B0BF-4B89-99BE-E0C6DBAE92C2}" name="Tabela8" displayName="Tabela8" ref="B21:C26" totalsRowShown="0" headerRowBorderDxfId="0" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F4D0B40F-B0BF-4B89-99BE-E0C6DBAE92C2}" name="Tabela8" displayName="Tabela8" ref="B21:C26" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="B21:C26" xr:uid="{F4D0B40F-B0BF-4B89-99BE-E0C6DBAE92C2}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{32F0D679-FD92-43A6-9CAC-DAAC1E15033B}" name="Frequência" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{95B8F6A5-73FA-446F-80A4-DCB781AC7D13}" name="Valor" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{32F0D679-FD92-43A6-9CAC-DAAC1E15033B}" name="Frequência" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{95B8F6A5-73FA-446F-80A4-DCB781AC7D13}" name="Valor" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2125,7 +2135,7 @@
   <dimension ref="A1:AF975"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2145,30 +2155,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
+      <c r="A1" s="56"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
       <c r="Y1" s="7"/>
       <c r="Z1" s="7"/>
       <c r="AA1" s="7"/>
@@ -2179,41 +2189,42 @@
       <c r="AF1" s="7"/>
     </row>
     <row r="2" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="56"/>
+      <c r="B2" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="48" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="48" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="M2" s="35" t="s">
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="36"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="35" t="s">
+      <c r="N2" s="47"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="36"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="35" t="s">
+      <c r="R2" s="47"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="V2" s="36"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="7"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="48"/>
+      <c r="X2" s="58"/>
       <c r="Y2" s="7"/>
       <c r="Z2" s="7"/>
       <c r="AA2" s="7"/>
@@ -2224,41 +2235,42 @@
       <c r="AF2" s="7"/>
     </row>
     <row r="3" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="46" t="s">
+      <c r="A3" s="56"/>
+      <c r="B3" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="38" t="s">
+      <c r="C3" s="55"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="38" t="s">
+      <c r="F3" s="42"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="39"/>
-      <c r="K3" s="40"/>
-      <c r="M3" s="38" t="s">
+      <c r="J3" s="42"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="39"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="38" t="s">
+      <c r="N3" s="42"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="39"/>
-      <c r="S3" s="40"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="38" t="s">
+      <c r="R3" s="42"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="V3" s="39"/>
-      <c r="W3" s="40"/>
-      <c r="X3" s="7"/>
+      <c r="V3" s="42"/>
+      <c r="W3" s="43"/>
+      <c r="X3" s="58"/>
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
       <c r="AA3" s="7"/>
@@ -2269,10 +2281,10 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="4" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="E4" s="8" t="s">
         <v>21</v>
       </c>
@@ -2282,7 +2294,7 @@
       <c r="G4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="5"/>
+      <c r="H4" s="57"/>
       <c r="I4" s="8" t="s">
         <v>21</v>
       </c>
@@ -2292,6 +2304,7 @@
       <c r="K4" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="L4" s="59"/>
       <c r="M4" s="8" t="s">
         <v>21</v>
       </c>
@@ -2301,7 +2314,7 @@
       <c r="O4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="5"/>
+      <c r="P4" s="57"/>
       <c r="Q4" s="8" t="s">
         <v>21</v>
       </c>
@@ -2311,7 +2324,7 @@
       <c r="S4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="7"/>
+      <c r="T4" s="58"/>
       <c r="U4" s="8" t="s">
         <v>21</v>
       </c>
@@ -2321,7 +2334,7 @@
       <c r="W4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="X4" s="7"/>
+      <c r="X4" s="58"/>
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
       <c r="AA4" s="7"/>
@@ -2332,12 +2345,12 @@
       <c r="AF4" s="7"/>
     </row>
     <row r="5" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="44" t="s">
+      <c r="A5" s="57"/>
+      <c r="B5" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="5"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="9">
         <v>16.3</v>
       </c>
@@ -2348,7 +2361,7 @@
         <f>ATAN(E5/F5)*180/PI()</f>
         <v>18.540986541795807</v>
       </c>
-      <c r="H5" s="5"/>
+      <c r="H5" s="57"/>
       <c r="I5" s="9">
         <v>18.5</v>
       </c>
@@ -2359,6 +2372,7 @@
         <f>ATAN(I5/J5)*180/PI()</f>
         <v>20.839749214080893</v>
       </c>
+      <c r="L5" s="59"/>
       <c r="M5" s="9">
         <v>12.7</v>
       </c>
@@ -2369,7 +2383,7 @@
         <f>ATAN(M5/N5)*180/PI()</f>
         <v>14.644867194730461</v>
       </c>
-      <c r="P5" s="5"/>
+      <c r="P5" s="57"/>
       <c r="Q5" s="9">
         <v>10.199999999999999</v>
       </c>
@@ -2380,7 +2394,7 @@
         <f>ATAN(Q5/R5)*180/PI()</f>
         <v>11.853004167743999</v>
       </c>
-      <c r="T5" s="7"/>
+      <c r="T5" s="58"/>
       <c r="U5" s="9">
         <v>14.1</v>
       </c>
@@ -2391,7 +2405,7 @@
         <f>ATAN(U5/V5)*180/PI()</f>
         <v>16.178683616279667</v>
       </c>
-      <c r="X5" s="7"/>
+      <c r="X5" s="58"/>
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
       <c r="AA5" s="7"/>
@@ -2402,43 +2416,44 @@
       <c r="AF5" s="7"/>
     </row>
     <row r="6" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="41" t="s">
+      <c r="D6" s="57"/>
+      <c r="E6" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="41" t="s">
+      <c r="F6" s="50"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="42"/>
-      <c r="K6" s="43"/>
-      <c r="M6" s="41" t="s">
+      <c r="J6" s="50"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="42"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="41" t="s">
+      <c r="N6" s="50"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="R6" s="42"/>
-      <c r="S6" s="43"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="41" t="s">
+      <c r="R6" s="50"/>
+      <c r="S6" s="51"/>
+      <c r="T6" s="58"/>
+      <c r="U6" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="V6" s="42"/>
-      <c r="W6" s="43"/>
-      <c r="X6" s="7"/>
+      <c r="V6" s="50"/>
+      <c r="W6" s="51"/>
+      <c r="X6" s="58"/>
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
       <c r="AA6" s="7"/>
@@ -2449,14 +2464,14 @@
       <c r="AF6" s="7"/>
     </row>
     <row r="7" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="A7" s="57"/>
       <c r="B7" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="11">
         <v>0.38069999999999998</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="57"/>
       <c r="E7" s="9" t="s">
         <v>12</v>
       </c>
@@ -2466,7 +2481,7 @@
       <c r="G7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="5"/>
+      <c r="H7" s="57"/>
       <c r="I7" s="9" t="s">
         <v>12</v>
       </c>
@@ -2476,6 +2491,7 @@
       <c r="K7" s="9" t="s">
         <v>14</v>
       </c>
+      <c r="L7" s="59"/>
       <c r="M7" s="12" t="s">
         <v>12</v>
       </c>
@@ -2485,7 +2501,7 @@
       <c r="O7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="P7" s="5"/>
+      <c r="P7" s="57"/>
       <c r="Q7" s="12" t="s">
         <v>12</v>
       </c>
@@ -2495,7 +2511,7 @@
       <c r="S7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="T7" s="7"/>
+      <c r="T7" s="58"/>
       <c r="U7" s="12" t="s">
         <v>12</v>
       </c>
@@ -2505,7 +2521,7 @@
       <c r="W7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="X7" s="7"/>
+      <c r="X7" s="58"/>
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
       <c r="AA7" s="7"/>
@@ -2516,14 +2532,14 @@
       <c r="AF7" s="7"/>
     </row>
     <row r="8" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="11">
         <v>7.6</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="56"/>
       <c r="E8" s="9">
         <v>1</v>
       </c>
@@ -2533,7 +2549,7 @@
       <c r="G8" s="31">
         <v>19.2</v>
       </c>
-      <c r="H8" s="34"/>
+      <c r="H8" s="60"/>
       <c r="I8" s="9">
         <v>1</v>
       </c>
@@ -2543,6 +2559,7 @@
       <c r="K8" s="16">
         <v>19.2</v>
       </c>
+      <c r="L8" s="59"/>
       <c r="M8" s="17">
         <v>1</v>
       </c>
@@ -2552,7 +2569,7 @@
       <c r="O8" s="19">
         <v>19.2</v>
       </c>
-      <c r="P8" s="5"/>
+      <c r="P8" s="57"/>
       <c r="Q8" s="17">
         <v>1</v>
       </c>
@@ -2562,7 +2579,7 @@
       <c r="S8" s="20">
         <v>19.2</v>
       </c>
-      <c r="T8" s="7"/>
+      <c r="T8" s="58"/>
       <c r="U8" s="17">
         <v>1</v>
       </c>
@@ -2572,7 +2589,7 @@
       <c r="W8" s="33">
         <v>19.399999999999999</v>
       </c>
-      <c r="X8" s="7"/>
+      <c r="X8" s="58"/>
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
       <c r="AA8" s="7"/>
@@ -2583,14 +2600,14 @@
       <c r="AF8" s="7"/>
     </row>
     <row r="9" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="11">
         <v>2.79</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="57"/>
       <c r="E9" s="9">
         <v>2</v>
       </c>
@@ -2600,7 +2617,7 @@
       <c r="G9" s="28">
         <v>19.2</v>
       </c>
-      <c r="H9" s="5"/>
+      <c r="H9" s="57"/>
       <c r="I9" s="9">
         <v>2</v>
       </c>
@@ -2610,6 +2627,7 @@
       <c r="K9" s="16">
         <v>19.3</v>
       </c>
+      <c r="L9" s="59"/>
       <c r="M9" s="17">
         <v>2</v>
       </c>
@@ -2619,7 +2637,7 @@
       <c r="O9" s="19">
         <v>19.3</v>
       </c>
-      <c r="P9" s="5"/>
+      <c r="P9" s="57"/>
       <c r="Q9" s="17">
         <v>2</v>
       </c>
@@ -2629,7 +2647,7 @@
       <c r="S9" s="20">
         <v>19.2</v>
       </c>
-      <c r="T9" s="7"/>
+      <c r="T9" s="58"/>
       <c r="U9" s="17">
         <v>2</v>
       </c>
@@ -2639,7 +2657,7 @@
       <c r="W9" s="20">
         <v>19.399999999999999</v>
       </c>
-      <c r="X9" s="7"/>
+      <c r="X9" s="58"/>
       <c r="Y9" s="7"/>
       <c r="Z9" s="7"/>
       <c r="AA9" s="7"/>
@@ -2650,14 +2668,14 @@
       <c r="AF9" s="7"/>
     </row>
     <row r="10" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+      <c r="A10" s="57"/>
       <c r="B10" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="22">
         <v>3.63</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="57"/>
       <c r="E10" s="9">
         <v>3</v>
       </c>
@@ -2667,7 +2685,7 @@
       <c r="G10" s="28">
         <v>19.2</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="56"/>
       <c r="I10" s="9">
         <v>3</v>
       </c>
@@ -2677,6 +2695,7 @@
       <c r="K10" s="16">
         <v>19.399999999999999</v>
       </c>
+      <c r="L10" s="59"/>
       <c r="M10" s="17">
         <v>3</v>
       </c>
@@ -2686,7 +2705,7 @@
       <c r="O10" s="19">
         <v>19.399999999999999</v>
       </c>
-      <c r="P10" s="5"/>
+      <c r="P10" s="57"/>
       <c r="Q10" s="17">
         <v>3</v>
       </c>
@@ -2696,7 +2715,7 @@
       <c r="S10" s="20">
         <v>19.3</v>
       </c>
-      <c r="T10" s="7"/>
+      <c r="T10" s="58"/>
       <c r="U10" s="17">
         <v>3</v>
       </c>
@@ -2706,7 +2725,7 @@
       <c r="W10" s="20">
         <v>19.399999999999999</v>
       </c>
-      <c r="X10" s="7"/>
+      <c r="X10" s="58"/>
       <c r="Y10" s="7"/>
       <c r="Z10" s="7"/>
       <c r="AA10" s="7"/>
@@ -2717,10 +2736,10 @@
       <c r="AF10" s="7"/>
     </row>
     <row r="11" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
       <c r="E11" s="9">
         <v>4</v>
       </c>
@@ -2730,7 +2749,7 @@
       <c r="G11" s="28">
         <v>19.3</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="56"/>
       <c r="I11" s="9">
         <v>4</v>
       </c>
@@ -2740,6 +2759,7 @@
       <c r="K11" s="16">
         <v>19.7</v>
       </c>
+      <c r="L11" s="59"/>
       <c r="M11" s="17">
         <v>4</v>
       </c>
@@ -2749,7 +2769,7 @@
       <c r="O11" s="19">
         <v>19.600000000000001</v>
       </c>
-      <c r="P11" s="5"/>
+      <c r="P11" s="57"/>
       <c r="Q11" s="17">
         <v>4</v>
       </c>
@@ -2759,7 +2779,7 @@
       <c r="S11" s="20">
         <v>19.399999999999999</v>
       </c>
-      <c r="T11" s="7"/>
+      <c r="T11" s="58"/>
       <c r="U11" s="17">
         <v>4</v>
       </c>
@@ -2769,7 +2789,7 @@
       <c r="W11" s="20">
         <v>19.600000000000001</v>
       </c>
-      <c r="X11" s="7"/>
+      <c r="X11" s="58"/>
       <c r="Y11" s="7"/>
       <c r="Z11" s="7"/>
       <c r="AA11" s="7"/>
@@ -2780,12 +2800,12 @@
       <c r="AF11" s="7"/>
     </row>
     <row r="12" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="52" t="s">
+      <c r="A12" s="57"/>
+      <c r="B12" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="5"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="57"/>
       <c r="E12" s="9">
         <v>5</v>
       </c>
@@ -2795,7 +2815,7 @@
       <c r="G12" s="28">
         <v>19.600000000000001</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="56"/>
       <c r="I12" s="9">
         <v>5</v>
       </c>
@@ -2805,6 +2825,7 @@
       <c r="K12" s="16">
         <v>20.3</v>
       </c>
+      <c r="L12" s="59"/>
       <c r="M12" s="17">
         <v>5</v>
       </c>
@@ -2814,7 +2835,7 @@
       <c r="O12" s="19">
         <v>20</v>
       </c>
-      <c r="P12" s="5"/>
+      <c r="P12" s="57"/>
       <c r="Q12" s="17">
         <v>5</v>
       </c>
@@ -2824,7 +2845,7 @@
       <c r="S12" s="20">
         <v>19.600000000000001</v>
       </c>
-      <c r="T12" s="7"/>
+      <c r="T12" s="58"/>
       <c r="U12" s="17">
         <v>5</v>
       </c>
@@ -2834,7 +2855,7 @@
       <c r="W12" s="20">
         <v>19.8</v>
       </c>
-      <c r="X12" s="7"/>
+      <c r="X12" s="58"/>
       <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
       <c r="AA12" s="7"/>
@@ -2845,12 +2866,12 @@
       <c r="AF12" s="7"/>
     </row>
     <row r="13" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="52" t="s">
+      <c r="A13" s="57"/>
+      <c r="B13" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="5"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="57"/>
       <c r="E13" s="9">
         <v>6</v>
       </c>
@@ -2860,7 +2881,7 @@
       <c r="G13" s="28">
         <v>20</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="56"/>
       <c r="I13" s="9">
         <v>6</v>
       </c>
@@ -2870,6 +2891,7 @@
       <c r="K13" s="16">
         <v>20.9</v>
       </c>
+      <c r="L13" s="59"/>
       <c r="M13" s="23">
         <v>6</v>
       </c>
@@ -2879,7 +2901,7 @@
       <c r="O13" s="19">
         <v>20.3</v>
       </c>
-      <c r="P13" s="5"/>
+      <c r="P13" s="57"/>
       <c r="Q13" s="23">
         <v>6</v>
       </c>
@@ -2889,7 +2911,7 @@
       <c r="S13" s="26">
         <v>19.8</v>
       </c>
-      <c r="T13" s="7"/>
+      <c r="T13" s="58"/>
       <c r="U13" s="23">
         <v>6</v>
       </c>
@@ -2899,7 +2921,7 @@
       <c r="W13" s="20">
         <v>20.2</v>
       </c>
-      <c r="X13" s="7"/>
+      <c r="X13" s="58"/>
       <c r="Y13" s="7"/>
       <c r="Z13" s="7"/>
       <c r="AA13" s="7"/>
@@ -2910,14 +2932,14 @@
       <c r="AF13" s="7"/>
     </row>
     <row r="14" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="53" t="s">
+      <c r="A14" s="57"/>
+      <c r="B14" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="58"/>
       <c r="E14" s="9">
         <v>7</v>
       </c>
@@ -2927,7 +2949,7 @@
       <c r="G14" s="28">
         <v>20.6</v>
       </c>
-      <c r="H14" s="5"/>
+      <c r="H14" s="57"/>
       <c r="I14" s="9">
         <v>7</v>
       </c>
@@ -2937,7 +2959,7 @@
       <c r="K14" s="28">
         <v>21.6</v>
       </c>
-      <c r="L14" s="7"/>
+      <c r="L14" s="58"/>
       <c r="M14" s="17">
         <v>7</v>
       </c>
@@ -2947,7 +2969,7 @@
       <c r="O14" s="19">
         <v>20.9</v>
       </c>
-      <c r="P14" s="5"/>
+      <c r="P14" s="57"/>
       <c r="Q14" s="17">
         <v>7</v>
       </c>
@@ -2957,7 +2979,7 @@
       <c r="S14" s="20">
         <v>20</v>
       </c>
-      <c r="T14" s="7"/>
+      <c r="T14" s="58"/>
       <c r="U14" s="17">
         <v>7</v>
       </c>
@@ -2967,7 +2989,7 @@
       <c r="W14" s="20">
         <v>20.7</v>
       </c>
-      <c r="X14" s="7"/>
+      <c r="X14" s="58"/>
       <c r="Y14" s="7"/>
       <c r="Z14" s="7"/>
       <c r="AA14" s="7"/>
@@ -2978,14 +3000,14 @@
       <c r="AF14" s="7"/>
     </row>
     <row r="15" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="49">
+      <c r="A15" s="57"/>
+      <c r="B15" s="34">
         <v>2</v>
       </c>
-      <c r="C15" s="50">
+      <c r="C15" s="35">
         <v>0.17</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="58"/>
       <c r="E15" s="9">
         <v>8</v>
       </c>
@@ -2995,7 +3017,7 @@
       <c r="G15" s="28">
         <v>21.3</v>
       </c>
-      <c r="H15" s="7"/>
+      <c r="H15" s="58"/>
       <c r="I15" s="9">
         <v>8</v>
       </c>
@@ -3005,7 +3027,7 @@
       <c r="K15" s="28">
         <v>22.8</v>
       </c>
-      <c r="L15" s="7"/>
+      <c r="L15" s="58"/>
       <c r="M15" s="17">
         <v>8</v>
       </c>
@@ -3015,7 +3037,7 @@
       <c r="O15" s="19">
         <v>21.4</v>
       </c>
-      <c r="P15" s="5"/>
+      <c r="P15" s="57"/>
       <c r="Q15" s="17">
         <v>8</v>
       </c>
@@ -3025,7 +3047,7 @@
       <c r="S15" s="20">
         <v>20.3</v>
       </c>
-      <c r="T15" s="7"/>
+      <c r="T15" s="58"/>
       <c r="U15" s="17">
         <v>8</v>
       </c>
@@ -3035,7 +3057,7 @@
       <c r="W15" s="20">
         <v>21.3</v>
       </c>
-      <c r="X15" s="7"/>
+      <c r="X15" s="58"/>
       <c r="Y15" s="7"/>
       <c r="Z15" s="7"/>
       <c r="AA15" s="7"/>
@@ -3046,14 +3068,14 @@
       <c r="AF15" s="7"/>
     </row>
     <row r="16" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="49">
+      <c r="A16" s="57"/>
+      <c r="B16" s="34">
         <v>7</v>
       </c>
-      <c r="C16" s="50">
+      <c r="C16" s="35">
         <v>0.19</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="58"/>
       <c r="E16" s="9">
         <v>9</v>
       </c>
@@ -3063,7 +3085,7 @@
       <c r="G16" s="28">
         <v>22.3</v>
       </c>
-      <c r="H16" s="7"/>
+      <c r="H16" s="58"/>
       <c r="I16" s="9">
         <v>9</v>
       </c>
@@ -3073,7 +3095,7 @@
       <c r="K16" s="28">
         <v>24.2</v>
       </c>
-      <c r="L16" s="7"/>
+      <c r="L16" s="58"/>
       <c r="M16" s="17">
         <v>9</v>
       </c>
@@ -3083,7 +3105,7 @@
       <c r="O16" s="19">
         <v>22</v>
       </c>
-      <c r="P16" s="5"/>
+      <c r="P16" s="57"/>
       <c r="Q16" s="17">
         <v>9</v>
       </c>
@@ -3093,6 +3115,7 @@
       <c r="S16" s="20">
         <v>20.7</v>
       </c>
+      <c r="T16" s="59"/>
       <c r="U16" s="17">
         <v>9</v>
       </c>
@@ -3102,7 +3125,7 @@
       <c r="W16" s="20">
         <v>21.9</v>
       </c>
-      <c r="X16" s="7"/>
+      <c r="X16" s="58"/>
       <c r="Y16" s="7"/>
       <c r="Z16" s="7"/>
       <c r="AA16" s="7"/>
@@ -3113,14 +3136,14 @@
       <c r="AF16" s="7"/>
     </row>
     <row r="17" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="49">
+      <c r="A17" s="57"/>
+      <c r="B17" s="34">
         <v>1</v>
       </c>
-      <c r="C17" s="50">
+      <c r="C17" s="35">
         <v>0.21</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="58"/>
       <c r="E17" s="9">
         <v>10</v>
       </c>
@@ -3130,7 +3153,7 @@
       <c r="G17" s="28">
         <v>23.3</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="58"/>
       <c r="I17" s="9">
         <v>10</v>
       </c>
@@ -3140,7 +3163,7 @@
       <c r="K17" s="30">
         <v>25.7</v>
       </c>
-      <c r="L17" s="7"/>
+      <c r="L17" s="58"/>
       <c r="M17" s="17">
         <v>10</v>
       </c>
@@ -3150,7 +3173,7 @@
       <c r="O17" s="19">
         <v>22.7</v>
       </c>
-      <c r="P17" s="5"/>
+      <c r="P17" s="57"/>
       <c r="Q17" s="17">
         <v>10</v>
       </c>
@@ -3160,6 +3183,7 @@
       <c r="S17" s="20">
         <v>21</v>
       </c>
+      <c r="T17" s="59"/>
       <c r="U17" s="23">
         <v>10</v>
       </c>
@@ -3169,7 +3193,7 @@
       <c r="W17" s="20">
         <v>22.8</v>
       </c>
-      <c r="X17" s="7"/>
+      <c r="X17" s="58"/>
       <c r="Y17" s="7"/>
       <c r="Z17" s="7"/>
       <c r="AA17" s="7"/>
@@ -3180,14 +3204,14 @@
       <c r="AF17" s="7"/>
     </row>
     <row r="18" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="49">
+      <c r="A18" s="56"/>
+      <c r="B18" s="34">
         <v>1</v>
       </c>
-      <c r="C18" s="50">
+      <c r="C18" s="35">
         <v>0.23</v>
       </c>
-      <c r="D18" s="7"/>
+      <c r="D18" s="58"/>
       <c r="E18" s="9">
         <v>11</v>
       </c>
@@ -3197,11 +3221,11 @@
       <c r="G18" s="28">
         <v>24.4</v>
       </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
       <c r="M18" s="17">
         <v>11</v>
       </c>
@@ -3211,7 +3235,7 @@
       <c r="O18" s="25">
         <v>23.5</v>
       </c>
-      <c r="P18" s="6"/>
+      <c r="P18" s="56"/>
       <c r="Q18" s="17">
         <v>11</v>
       </c>
@@ -3221,6 +3245,7 @@
       <c r="S18" s="20">
         <v>21.4</v>
       </c>
+      <c r="T18" s="59"/>
       <c r="U18" s="17">
         <v>11</v>
       </c>
@@ -3230,7 +3255,7 @@
       <c r="W18" s="26">
         <v>23.2</v>
       </c>
-      <c r="X18" s="7"/>
+      <c r="X18" s="58"/>
       <c r="Y18" s="7"/>
       <c r="Z18" s="7"/>
       <c r="AA18" s="7"/>
@@ -3241,16 +3266,16 @@
       <c r="AF18" s="7"/>
     </row>
     <row r="19" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="55">
+      <c r="A19" s="56"/>
+      <c r="B19" s="39">
         <f>SUM(B15:B18)</f>
         <v>11</v>
       </c>
-      <c r="C19" s="56">
+      <c r="C19" s="40">
         <f>(B15*C15+B16*C16+B17*C17+C18*B18)/B19</f>
         <v>0.19181818181818186</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="58"/>
       <c r="E19" s="9">
         <v>12</v>
       </c>
@@ -3260,11 +3285,11 @@
       <c r="G19" s="28">
         <v>25.7</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
       <c r="M19" s="23">
         <v>12</v>
       </c>
@@ -3274,7 +3299,7 @@
       <c r="O19" s="19">
         <v>24.4</v>
       </c>
-      <c r="P19" s="6"/>
+      <c r="P19" s="56"/>
       <c r="Q19" s="23">
         <v>12</v>
       </c>
@@ -3284,6 +3309,7 @@
       <c r="S19" s="20">
         <v>21.9</v>
       </c>
+      <c r="T19" s="59"/>
       <c r="U19" s="17">
         <v>12</v>
       </c>
@@ -3293,7 +3319,7 @@
       <c r="W19" s="20">
         <v>24.8</v>
       </c>
-      <c r="X19" s="7"/>
+      <c r="X19" s="58"/>
       <c r="Y19" s="7"/>
       <c r="Z19" s="7"/>
       <c r="AA19" s="7"/>
@@ -3304,12 +3330,12 @@
       <c r="AF19" s="7"/>
     </row>
     <row r="20" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="52" t="s">
+      <c r="A20" s="57"/>
+      <c r="B20" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="52"/>
-      <c r="D20" s="7"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="58"/>
       <c r="E20" s="9">
         <v>13</v>
       </c>
@@ -3319,11 +3345,11 @@
       <c r="G20" s="16">
         <v>27.4</v>
       </c>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="58"/>
       <c r="M20" s="17">
         <v>13</v>
       </c>
@@ -3333,7 +3359,7 @@
       <c r="O20" s="25">
         <v>25.4</v>
       </c>
-      <c r="P20" s="5"/>
+      <c r="P20" s="57"/>
       <c r="Q20" s="17">
         <v>13</v>
       </c>
@@ -3343,6 +3369,7 @@
       <c r="S20" s="20">
         <v>22.4</v>
       </c>
+      <c r="T20" s="59"/>
       <c r="U20" s="17">
         <v>13</v>
       </c>
@@ -3352,7 +3379,7 @@
       <c r="W20" s="20">
         <v>25.9</v>
       </c>
-      <c r="X20" s="7"/>
+      <c r="X20" s="58"/>
       <c r="Y20" s="7"/>
       <c r="Z20" s="7"/>
       <c r="AA20" s="7"/>
@@ -3363,23 +3390,26 @@
       <c r="AF20" s="7"/>
     </row>
     <row r="21" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="53" t="s">
+      <c r="A21" s="57"/>
+      <c r="B21" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="5"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="58"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="58"/>
+      <c r="N21" s="58"/>
+      <c r="O21" s="58"/>
+      <c r="P21" s="57"/>
       <c r="Q21" s="17">
         <v>14</v>
       </c>
@@ -3389,7 +3419,11 @@
       <c r="S21" s="20">
         <v>22.9</v>
       </c>
-      <c r="X21" s="7"/>
+      <c r="T21" s="59"/>
+      <c r="U21" s="59"/>
+      <c r="V21" s="59"/>
+      <c r="W21" s="59"/>
+      <c r="X21" s="58"/>
       <c r="Y21" s="7"/>
       <c r="Z21" s="7"/>
       <c r="AA21" s="7"/>
@@ -3400,23 +3434,26 @@
       <c r="AF21" s="7"/>
     </row>
     <row r="22" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="49">
+      <c r="A22" s="57"/>
+      <c r="B22" s="34">
         <v>2</v>
       </c>
-      <c r="C22" s="50">
+      <c r="C22" s="35">
         <v>0.22500000000000001</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="5"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="58"/>
+      <c r="K22" s="58"/>
+      <c r="L22" s="58"/>
+      <c r="M22" s="58"/>
+      <c r="N22" s="58"/>
+      <c r="O22" s="58"/>
+      <c r="P22" s="57"/>
       <c r="Q22" s="17">
         <v>15</v>
       </c>
@@ -3426,7 +3463,11 @@
       <c r="S22" s="20">
         <v>23.4</v>
       </c>
-      <c r="X22" s="7"/>
+      <c r="T22" s="59"/>
+      <c r="U22" s="59"/>
+      <c r="V22" s="59"/>
+      <c r="W22" s="59"/>
+      <c r="X22" s="58"/>
       <c r="Y22" s="7"/>
       <c r="Z22" s="7"/>
       <c r="AA22" s="7"/>
@@ -3437,22 +3478,26 @@
       <c r="AF22" s="7"/>
     </row>
     <row r="23" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="49">
+      <c r="A23" s="57"/>
+      <c r="B23" s="34">
         <v>5</v>
       </c>
-      <c r="C23" s="50">
+      <c r="C23" s="35">
         <v>0.27500000000000002</v>
       </c>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="5"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="58"/>
+      <c r="N23" s="58"/>
+      <c r="O23" s="58"/>
+      <c r="P23" s="57"/>
       <c r="Q23" s="23">
         <v>16</v>
       </c>
@@ -3462,7 +3507,11 @@
       <c r="S23" s="26">
         <v>24</v>
       </c>
-      <c r="X23" s="7"/>
+      <c r="T23" s="59"/>
+      <c r="U23" s="59"/>
+      <c r="V23" s="59"/>
+      <c r="W23" s="59"/>
+      <c r="X23" s="58"/>
       <c r="Y23" s="7"/>
       <c r="Z23" s="7"/>
       <c r="AA23" s="7"/>
@@ -3473,23 +3522,34 @@
       <c r="AF23" s="7"/>
     </row>
     <row r="24" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="49">
+      <c r="A24" s="56"/>
+      <c r="B24" s="34">
         <v>3</v>
       </c>
-      <c r="C24" s="51">
+      <c r="C24" s="36">
         <v>0.32500000000000001</v>
       </c>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="5"/>
-      <c r="X24" s="7"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="58"/>
+      <c r="O24" s="58"/>
+      <c r="P24" s="57"/>
+      <c r="Q24" s="59"/>
+      <c r="R24" s="59"/>
+      <c r="S24" s="59"/>
+      <c r="T24" s="59"/>
+      <c r="U24" s="59"/>
+      <c r="V24" s="59"/>
+      <c r="W24" s="59"/>
+      <c r="X24" s="58"/>
       <c r="Y24" s="7"/>
       <c r="Z24" s="7"/>
       <c r="AA24" s="7"/>
@@ -3500,23 +3560,34 @@
       <c r="AF24" s="7"/>
     </row>
     <row r="25" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="49">
+      <c r="A25" s="56"/>
+      <c r="B25" s="34">
         <v>1</v>
       </c>
-      <c r="C25" s="51">
+      <c r="C25" s="36">
         <v>0.375</v>
       </c>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="5"/>
-      <c r="X25" s="7"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="58"/>
+      <c r="P25" s="57"/>
+      <c r="Q25" s="59"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="59"/>
+      <c r="T25" s="59"/>
+      <c r="U25" s="59"/>
+      <c r="V25" s="59"/>
+      <c r="W25" s="59"/>
+      <c r="X25" s="58"/>
       <c r="Y25" s="7"/>
       <c r="Z25" s="7"/>
       <c r="AA25" s="7"/>
@@ -3527,23 +3598,36 @@
       <c r="AF25" s="7"/>
     </row>
     <row r="26" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="55">
+      <c r="A26" s="56"/>
+      <c r="B26" s="39">
         <f>SUM(B22:B25)</f>
         <v>11</v>
       </c>
-      <c r="C26" s="56">
+      <c r="C26" s="40">
         <f>(B22*C22+B23*C23+B24*C24+C25*B25)/B26</f>
         <v>0.28863636363636364</v>
       </c>
-      <c r="H26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="5"/>
-      <c r="X26" s="7"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="58"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="58"/>
+      <c r="N26" s="58"/>
+      <c r="O26" s="58"/>
+      <c r="P26" s="57"/>
+      <c r="Q26" s="59"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="59"/>
+      <c r="T26" s="59"/>
+      <c r="U26" s="59"/>
+      <c r="V26" s="59"/>
+      <c r="W26" s="59"/>
+      <c r="X26" s="58"/>
       <c r="Y26" s="7"/>
       <c r="Z26" s="7"/>
       <c r="AA26" s="7"/>
@@ -3554,15 +3638,30 @@
       <c r="AF26" s="7"/>
     </row>
     <row r="27" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="H27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="5"/>
-      <c r="X27" s="7"/>
+      <c r="A27" s="56"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="58"/>
+      <c r="N27" s="58"/>
+      <c r="O27" s="58"/>
+      <c r="P27" s="57"/>
+      <c r="Q27" s="59"/>
+      <c r="R27" s="59"/>
+      <c r="S27" s="59"/>
+      <c r="T27" s="59"/>
+      <c r="U27" s="59"/>
+      <c r="V27" s="59"/>
+      <c r="W27" s="59"/>
+      <c r="X27" s="58"/>
       <c r="Y27" s="7"/>
       <c r="Z27" s="7"/>
       <c r="AA27" s="7"/>
@@ -9136,11 +9235,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B20:C20"/>
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="U3:W3"/>
     <mergeCell ref="U6:W6"/>
@@ -9157,10 +9251,15 @@
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="Q3:S3"/>
     <mergeCell ref="I2:K2"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="8">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -9168,6 +9267,7 @@
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>